<commit_message>
Added genre and comments controllers
</commit_message>
<xml_diff>
--- a/DescriptionAPI.xlsx
+++ b/DescriptionAPI.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="72">
   <si>
     <t>MUS</t>
   </si>
@@ -156,18 +156,9 @@
     <t>Просмотр списка коминтариев (авторизированный пользователь)</t>
   </si>
   <si>
-    <t>GENRES</t>
-  </si>
-  <si>
-    <t>/genre/</t>
-  </si>
-  <si>
     <t>Добавление жанра (администратор)</t>
   </si>
   <si>
-    <t>(id - идентификатор жанра) - Просмотр конкретного жанра (авторизированный пользователь)</t>
-  </si>
-  <si>
     <t>(id - идентификатор жанра) - Изменение жанра (администратор)</t>
   </si>
   <si>
@@ -216,12 +207,6 @@
     <t>Добавление подписки  (авторизированный пользователь)</t>
   </si>
   <si>
-    <t>(id - идентификатор подписки) - Просмотр конкретного подписки  (авторизированный пользователь)</t>
-  </si>
-  <si>
-    <t>(id - идентификатор подписки) - Изменение подписки (авторизированный пользователь)</t>
-  </si>
-  <si>
     <t>(id - идентификатор подписки) - Удаление подписки  (авторизированный пользователь)</t>
   </si>
   <si>
@@ -241,6 +226,15 @@
   </si>
   <si>
     <t>/playlists/allPlaylists</t>
+  </si>
+  <si>
+    <t>GENRE</t>
+  </si>
+  <si>
+    <t>/genre/add</t>
+  </si>
+  <si>
+    <t>/genre/all</t>
   </si>
 </sst>
 </file>
@@ -594,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -666,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -683,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -727,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -902,7 +896,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B38" s="6"/>
     </row>
@@ -911,139 +905,139 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="6"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="D52" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="6"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" t="s">
         <v>62</v>
-      </c>
-      <c r="D53" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,63 +1045,66 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
         <v>63</v>
       </c>
-      <c r="D54" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C55" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,93 +1113,57 @@
         <v>2</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-    </row>
-    <row r="70" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="D70" s="1"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="2"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
-    </row>
-    <row r="78" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="D78" s="1"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="2"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+    </row>
+    <row r="67" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D67" s="1"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+    </row>
+    <row r="75" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>